<commit_message>
Updates made by me and Eric Menendez
Some of these changes were made a while ago by me and some were made
recently (April 1, 2014 - no fooling) by Eric Menendez.
</commit_message>
<xml_diff>
--- a/Tools/Tables/LandCover_Class.xlsx
+++ b/Tools/Tables/LandCover_Class.xlsx
@@ -19,12 +19,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
-    <t>LCCC</t>
-  </si>
-  <si>
-    <t>DESCRIPTIO</t>
-  </si>
-  <si>
     <t>Open Water</t>
   </si>
   <si>
@@ -112,7 +106,13 @@
     <t>Estuarine Aquatic Bed</t>
   </si>
   <si>
-    <t>Walk_Impd</t>
+    <t>LAND COVER CODE</t>
+  </si>
+  <si>
+    <t>DESCRIPTION</t>
+  </si>
+  <si>
+    <t>IMPEDANCE</t>
   </si>
 </sst>
 </file>
@@ -600,7 +600,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -615,6 +615,9 @@
     </xf>
     <xf numFmtId="1" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -960,23 +963,23 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection sqref="A1:C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="32.28515625" style="2" customWidth="1"/>
     <col min="3" max="3" width="16.7109375" style="4" customWidth="1"/>
     <col min="4" max="4" width="10.85546875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
+    <row r="1" spans="1:4" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>29</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>31</v>
@@ -988,7 +991,7 @@
         <v>11</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C2" s="3">
         <v>99</v>
@@ -999,7 +1002,7 @@
         <v>12</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C3" s="3">
         <v>80</v>
@@ -1010,7 +1013,7 @@
         <v>21</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C4" s="3">
         <v>20</v>
@@ -1021,7 +1024,7 @@
         <v>22</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C5" s="3">
         <v>20</v>
@@ -1032,7 +1035,7 @@
         <v>23</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C6" s="3">
         <v>30</v>
@@ -1043,7 +1046,7 @@
         <v>24</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C7" s="3">
         <v>40</v>
@@ -1054,7 +1057,7 @@
         <v>31</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C8" s="3">
         <v>60</v>
@@ -1065,7 +1068,7 @@
         <v>32</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C9" s="3">
         <v>70</v>
@@ -1076,7 +1079,7 @@
         <v>41</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C10" s="3">
         <v>50</v>
@@ -1087,7 +1090,7 @@
         <v>42</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C11" s="3">
         <v>50</v>
@@ -1098,7 +1101,7 @@
         <v>43</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C12" s="3">
         <v>50</v>
@@ -1109,7 +1112,7 @@
         <v>51</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C13" s="3">
         <v>75</v>
@@ -1120,7 +1123,7 @@
         <v>52</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C14" s="3">
         <v>75</v>
@@ -1131,7 +1134,7 @@
         <v>71</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C15" s="3">
         <v>50</v>
@@ -1142,7 +1145,7 @@
         <v>72</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C16" s="3">
         <v>50</v>
@@ -1153,7 +1156,7 @@
         <v>73</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C17" s="3">
         <v>20</v>
@@ -1164,7 +1167,7 @@
         <v>74</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C18" s="3">
         <v>20</v>
@@ -1175,7 +1178,7 @@
         <v>81</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C19" s="3">
         <v>20</v>
@@ -1186,7 +1189,7 @@
         <v>82</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C20" s="3">
         <v>30</v>
@@ -1197,7 +1200,7 @@
         <v>90</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C21" s="3">
         <v>80</v>
@@ -1208,7 +1211,7 @@
         <v>91</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C22" s="3">
         <v>80</v>
@@ -1219,7 +1222,7 @@
         <v>92</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C23" s="3">
         <v>80</v>
@@ -1230,7 +1233,7 @@
         <v>93</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C24" s="3">
         <v>80</v>
@@ -1241,7 +1244,7 @@
         <v>94</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C25" s="3">
         <v>80</v>
@@ -1252,7 +1255,7 @@
         <v>95</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C26" s="3">
         <v>80</v>
@@ -1263,7 +1266,7 @@
         <v>96</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C27" s="3">
         <v>80</v>
@@ -1274,7 +1277,7 @@
         <v>97</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C28" s="3">
         <v>80</v>
@@ -1285,7 +1288,7 @@
         <v>98</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C29" s="3">
         <v>99</v>
@@ -1296,7 +1299,7 @@
         <v>99</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C30" s="3">
         <v>99</v>

</xml_diff>

<commit_message>
Updates to some scripts
Some updates were made to SARForms and some scripts
</commit_message>
<xml_diff>
--- a/Tools/Tables/LandCover_Class.xlsx
+++ b/Tools/Tables/LandCover_Class.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MapSAR_Ex\Tools\Tables\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="360" yWindow="345" windowWidth="24675" windowHeight="12555"/>
   </bookViews>
@@ -10,7 +15,7 @@
     <sheet name="LandCover_Class" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Database">LandCover_Class!$A$1:$D$30</definedName>
+    <definedName name="_xlnm.Database">LandCover_Class!$A$1:$C$30</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -600,7 +605,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -617,6 +622,9 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -669,6 +677,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -716,7 +727,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -751,7 +762,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -960,21 +971,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C30"/>
+      <selection activeCell="D1" sqref="D1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="32.28515625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="29" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>29</v>
       </c>
@@ -984,9 +994,8 @@
       <c r="C1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="6"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>11</v>
       </c>
@@ -997,7 +1006,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>12</v>
       </c>
@@ -1005,10 +1014,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="3">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>21</v>
       </c>
@@ -1016,10 +1025,10 @@
         <v>2</v>
       </c>
       <c r="C4" s="3">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>22</v>
       </c>
@@ -1027,10 +1036,10 @@
         <v>3</v>
       </c>
       <c r="C5" s="3">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>23</v>
       </c>
@@ -1038,10 +1047,10 @@
         <v>4</v>
       </c>
       <c r="C6" s="3">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>24</v>
       </c>
@@ -1049,10 +1058,10 @@
         <v>5</v>
       </c>
       <c r="C7" s="3">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>31</v>
       </c>
@@ -1060,10 +1069,10 @@
         <v>6</v>
       </c>
       <c r="C8" s="3">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>32</v>
       </c>
@@ -1071,10 +1080,10 @@
         <v>7</v>
       </c>
       <c r="C9" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>41</v>
       </c>
@@ -1082,10 +1091,10 @@
         <v>8</v>
       </c>
       <c r="C10" s="3">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>42</v>
       </c>
@@ -1096,7 +1105,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>43</v>
       </c>
@@ -1104,10 +1113,10 @@
         <v>10</v>
       </c>
       <c r="C12" s="3">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>51</v>
       </c>
@@ -1115,10 +1124,10 @@
         <v>11</v>
       </c>
       <c r="C13" s="3">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>52</v>
       </c>
@@ -1126,10 +1135,10 @@
         <v>12</v>
       </c>
       <c r="C14" s="3">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>71</v>
       </c>
@@ -1137,10 +1146,10 @@
         <v>13</v>
       </c>
       <c r="C15" s="3">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>72</v>
       </c>
@@ -1148,7 +1157,7 @@
         <v>14</v>
       </c>
       <c r="C16" s="3">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -1170,7 +1179,7 @@
         <v>16</v>
       </c>
       <c r="C18" s="3">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -1181,7 +1190,7 @@
         <v>17</v>
       </c>
       <c r="C19" s="3">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -1261,11 +1270,11 @@
         <v>80</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>96</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="9" t="s">
         <v>25</v>
       </c>
       <c r="C27" s="3">

</xml_diff>